<commit_message>
outputs with min and max
</commit_message>
<xml_diff>
--- a/outputs/outputWithoutFXD.xlsx
+++ b/outputs/outputWithoutFXD.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Measure</t>
   </si>
@@ -29,57 +29,30 @@
     <t>SD</t>
   </si>
   <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
     <t>Observations</t>
   </si>
   <si>
     <t>SIZE</t>
   </si>
   <si>
-    <t>7.96067307692308</t>
-  </si>
-  <si>
-    <t>8.2</t>
-  </si>
-  <si>
-    <t>1.68412707614019</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
-    <t>4856.55865384615</t>
-  </si>
-  <si>
-    <t>4864.42741456534</t>
-  </si>
-  <si>
     <t>FSD</t>
   </si>
   <si>
     <t>FSTS</t>
   </si>
   <si>
-    <t>0.496267882903846</t>
-  </si>
-  <si>
-    <t>0.43</t>
-  </si>
-  <si>
-    <t>0.238911874629314</t>
-  </si>
-  <si>
     <t>Tobin's Q</t>
   </si>
   <si>
-    <t>2.52451923076923</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>3.1299656872736</t>
-  </si>
-  <si>
     <t>FXD</t>
   </si>
   <si>
@@ -92,78 +65,24 @@
     <t>R&amp;D/sales</t>
   </si>
   <si>
-    <t>0.666866538461538</t>
-  </si>
-  <si>
-    <t>0.000215</t>
-  </si>
-  <si>
-    <t>3.08713698742661</t>
-  </si>
-  <si>
     <t>Leverage</t>
   </si>
   <si>
-    <t>0.59425</t>
-  </si>
-  <si>
-    <t>0.315</t>
-  </si>
-  <si>
-    <t>0.869354606612765</t>
-  </si>
-  <si>
     <t>Quick ratio</t>
   </si>
   <si>
-    <t>0.880586538461538</t>
-  </si>
-  <si>
-    <t>0.22</t>
-  </si>
-  <si>
-    <t>1.53913201242184</t>
-  </si>
-  <si>
     <t>Capex/sales</t>
   </si>
   <si>
-    <t>0.803884615384615</t>
-  </si>
-  <si>
-    <t>0.017</t>
-  </si>
-  <si>
-    <t>5.35346201805805</t>
-  </si>
-  <si>
     <t>ROA </t>
   </si>
   <si>
-    <t>0.0469615384615385</t>
-  </si>
-  <si>
-    <t>0.0725</t>
-  </si>
-  <si>
-    <t>0.180762028998646</t>
-  </si>
-  <si>
     <t>DD</t>
   </si>
   <si>
-    <t>0.769230769230769</t>
-  </si>
-  <si>
-    <t>0.423365371151993</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>0.230769230769231</t>
-  </si>
-  <si>
     <t>DE</t>
   </si>
   <si>
@@ -171,15 +90,6 @@
   </si>
   <si>
     <t>Tobin's Q (ln)</t>
-  </si>
-  <si>
-    <t>0.562616840653801</t>
-  </si>
-  <si>
-    <t>0.336472236621213</t>
-  </si>
-  <si>
-    <t>0.741403114779839</t>
   </si>
 </sst>
 </file>
@@ -276,10 +186,10 @@
     <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="11" sqref="B2:B3 B5:F6 B10:B16 B19:F19 C2 C10:C14 D2:E3 D10:D16 E14 F2 F10:F14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -287,8 +197,10 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2908163265306"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9234693877551"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.9336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9642857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,44 +219,62 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
+      <c r="B2" s="0" t="n">
+        <v>7.96067307692308</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1.68412707614019</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>4856.55865384615</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>3978</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
+      <c r="D3" s="0" t="n">
+        <v>4864.42741456534</v>
       </c>
       <c r="E3" s="0" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>18160</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -356,46 +286,64 @@
         <v>0</v>
       </c>
       <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.496267882903846</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.238911874629314</v>
       </c>
       <c r="E5" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2.52451923076923</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>3.1299656872736</v>
       </c>
       <c r="E6" s="0" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>22.81</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -407,12 +355,18 @@
         <v>0</v>
       </c>
       <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -424,12 +378,18 @@
         <v>0</v>
       </c>
       <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -441,131 +401,179 @@
         <v>0</v>
       </c>
       <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.666866538461538</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.000215</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>3.08713698742661</v>
       </c>
       <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>19.63</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.59425</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.315</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.869354606612765</v>
       </c>
       <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>35</v>
+        <v>17</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.880586538461538</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1.53913201242184</v>
       </c>
       <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.803884615384615</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>5.35346201805805</v>
       </c>
       <c r="E13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>53.36</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>43</v>
+        <v>19</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0.0469615384615385</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.0725</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0.180762028998646</v>
       </c>
       <c r="E14" s="0" t="n">
+        <v>-0.72</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>45</v>
+        <v>20</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.769230769230769</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>46</v>
+      <c r="D15" s="0" t="n">
+        <v>0.423365371151993</v>
       </c>
       <c r="E15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>48</v>
+        <v>21</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.230769230769231</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>46</v>
+      <c r="D16" s="0" t="n">
+        <v>0.423365371151993</v>
       </c>
       <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -577,12 +585,18 @@
         <v>0</v>
       </c>
       <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -594,23 +608,35 @@
         <v>0</v>
       </c>
       <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>54</v>
+        <v>24</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.562616840653801</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.336472236621213</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0.741403114779839</v>
       </c>
       <c r="E19" s="0" t="n">
+        <v>-0.415515443961666</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>3.1271990362963</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>104</v>
       </c>
     </row>

</xml_diff>